<commit_message>
Fixed some missing / incorrect fields in Beam channel
I went through more data from the SD card and updated some fields that have data.  I am not sure what some of it is.
</commit_message>
<xml_diff>
--- a/Decoder Ring.xlsx
+++ b/Decoder Ring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DRossman\Downloads\DataFlow-main\DataFlow-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EC8380-9572-4929-875E-26EE8A639854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1B32E68-94C3-4C9E-AA43-2AA2BBF0CF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60405" yWindow="-6105" windowWidth="25830" windowHeight="17940" activeTab="5" xr2:uid="{D3089677-3F36-4795-9B26-0BDE8E67A95B}"/>
+    <workbookView xWindow="57720" yWindow="-6570" windowWidth="21255" windowHeight="20670" activeTab="5" xr2:uid="{D3089677-3F36-4795-9B26-0BDE8E67A95B}"/>
   </bookViews>
   <sheets>
     <sheet name="Capture4 Raw Data" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2182" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2196" uniqueCount="640">
   <si>
     <t>Starting - B11 @ 70keV - magnet current = 248, extractV = 70.2, DF mag curr = 24.667, amu = 11, extrv = 71.138</t>
   </si>
@@ -1312,12 +1312,6 @@
     <t>1. Summing all of the columns AFTER the channel ID (after byte 4) to the column before the check sum.</t>
   </si>
   <si>
-    <t>2. Taking the mod of the sum and 255 and subtracting the floor of the sum</t>
-  </si>
-  <si>
-    <t>3. If this value is negative, add 256.</t>
-  </si>
-  <si>
     <t>Magnet current follows the same formula as Beam Energy.</t>
   </si>
   <si>
@@ -1720,21 +1714,6 @@
     <t>Accel Suppression Voltage - 64 = 0.002</t>
   </si>
   <si>
-    <t>34 to 37</t>
-  </si>
-  <si>
-    <t>98 to 113</t>
-  </si>
-  <si>
-    <t>122 to 125</t>
-  </si>
-  <si>
-    <t>134 to 149</t>
-  </si>
-  <si>
-    <t>158 to 165</t>
-  </si>
-  <si>
     <t>Vaporizer Status - 0 to 15 = Off, 16 - 31 = On, 32 - ? = Cool, but it cycles back to Off?  When I captured data it was at 64.</t>
   </si>
   <si>
@@ -1940,6 +1919,51 @@
   </si>
   <si>
     <t>Plus Ten 3 - 64 = 2</t>
+  </si>
+  <si>
+    <t>134 to 137</t>
+  </si>
+  <si>
+    <t>MSB Signal 26b</t>
+  </si>
+  <si>
+    <t>2. Taking the mod of the sum and 255 and subtracting the floor of the sum divided by 255</t>
+  </si>
+  <si>
+    <t>3. If this value is negative, add 256 until it is not negative.</t>
+  </si>
+  <si>
+    <t>MSB Signal 7b</t>
+  </si>
+  <si>
+    <t>MSB Signal 22b</t>
+  </si>
+  <si>
+    <t>MSB Signal 22c</t>
+  </si>
+  <si>
+    <t>MSB Signal 22d</t>
+  </si>
+  <si>
+    <t>MSB Signal 22e</t>
+  </si>
+  <si>
+    <t>MSB Signal 24b</t>
+  </si>
+  <si>
+    <t>E.S. Aperture V (this is 26b because I found it late… too lazy to renumber - always zero in the data that I have collected)</t>
+  </si>
+  <si>
+    <t>MSB Signal 26c</t>
+  </si>
+  <si>
+    <t>142 to 145</t>
+  </si>
+  <si>
+    <t>MSB Signal 28b</t>
+  </si>
+  <si>
+    <t>152 to 165</t>
   </si>
 </sst>
 </file>
@@ -68417,15 +68441,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D21FFDC-D4C9-49CE-97EF-F91F73D1EB22}">
-  <dimension ref="A1:J202"/>
+  <dimension ref="A1:J209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B163" sqref="B163"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G150" sqref="G150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -68440,7 +68464,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="B5" t="s">
         <v>300</v>
@@ -68587,7 +68611,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -68597,7 +68621,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="B15" t="s">
         <v>300</v>
@@ -68726,7 +68750,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -68741,12 +68765,12 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>422</v>
+        <v>627</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>423</v>
+        <v>628</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="21" x14ac:dyDescent="0.4">
@@ -68801,7 +68825,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -68811,13 +68835,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="B46" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
       <c r="D46" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -68836,10 +68860,10 @@
         <v>401</v>
       </c>
       <c r="B48" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="D48" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -68849,34 +68873,34 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B53">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="C53" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B54">
         <v>66</v>
       </c>
       <c r="C54" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -68891,22 +68915,22 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B65">
         <v>1.3332999999999999</v>
@@ -68914,7 +68938,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B66">
         <v>64</v>
@@ -68922,7 +68946,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -68932,32 +68956,32 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B78">
         <v>3.125038028597505E-2</v>
@@ -68965,7 +68989,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B79">
         <v>61</v>
@@ -68973,7 +68997,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
@@ -69025,7 +69049,7 @@
         <v>4</v>
       </c>
       <c r="D87" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
@@ -69039,7 +69063,7 @@
         <v>18</v>
       </c>
       <c r="D88" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
@@ -69135,10 +69159,10 @@
         <v>357</v>
       </c>
       <c r="C97" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D97" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -69196,7 +69220,7 @@
         <v>5</v>
       </c>
       <c r="D102" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -69240,7 +69264,7 @@
         <v>255</v>
       </c>
       <c r="D106" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="21" x14ac:dyDescent="0.4">
@@ -69297,7 +69321,7 @@
         <v>5</v>
       </c>
       <c r="D114" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
@@ -69311,7 +69335,7 @@
         <v>200</v>
       </c>
       <c r="D115" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
@@ -69330,10 +69354,10 @@
         <v>6</v>
       </c>
       <c r="B117" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C117" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
@@ -69341,10 +69365,10 @@
         <v>10</v>
       </c>
       <c r="B118" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C118" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
@@ -69352,10 +69376,10 @@
         <v>14</v>
       </c>
       <c r="B119" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C119" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
@@ -69363,10 +69387,10 @@
         <v>18</v>
       </c>
       <c r="B120" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C120" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -69374,10 +69398,10 @@
         <v>22</v>
       </c>
       <c r="B121" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C121" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
@@ -69385,10 +69409,10 @@
         <v>26</v>
       </c>
       <c r="B122" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C122" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
@@ -69396,21 +69420,21 @@
         <v>30</v>
       </c>
       <c r="B123" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C123" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>558</v>
+      <c r="A124">
+        <v>34</v>
       </c>
       <c r="B124" t="s">
-        <v>354</v>
-      </c>
-      <c r="C124">
-        <v>0</v>
+        <v>629</v>
+      </c>
+      <c r="C124" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
@@ -69418,10 +69442,10 @@
         <v>38</v>
       </c>
       <c r="B125" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C125" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
@@ -69429,10 +69453,10 @@
         <v>42</v>
       </c>
       <c r="B126" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C126" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
@@ -69440,10 +69464,10 @@
         <v>46</v>
       </c>
       <c r="B127" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C127" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
@@ -69451,10 +69475,10 @@
         <v>50</v>
       </c>
       <c r="B128" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C128" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
@@ -69462,10 +69486,10 @@
         <v>54</v>
       </c>
       <c r="B129" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C129" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
@@ -69473,10 +69497,10 @@
         <v>58</v>
       </c>
       <c r="B130" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C130" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -69484,10 +69508,10 @@
         <v>62</v>
       </c>
       <c r="B131" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C131" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
@@ -69495,10 +69519,10 @@
         <v>66</v>
       </c>
       <c r="B132" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C132" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
@@ -69506,10 +69530,10 @@
         <v>70</v>
       </c>
       <c r="B133" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C133" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
@@ -69517,10 +69541,10 @@
         <v>74</v>
       </c>
       <c r="B134" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C134" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
@@ -69528,10 +69552,10 @@
         <v>78</v>
       </c>
       <c r="B135" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C135" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
@@ -69539,10 +69563,10 @@
         <v>82</v>
       </c>
       <c r="B136" t="s">
+        <v>524</v>
+      </c>
+      <c r="C136" t="s">
         <v>526</v>
-      </c>
-      <c r="C136" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
@@ -69550,10 +69574,10 @@
         <v>86</v>
       </c>
       <c r="B137" t="s">
+        <v>525</v>
+      </c>
+      <c r="C137" t="s">
         <v>527</v>
-      </c>
-      <c r="C137" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
@@ -69561,10 +69585,10 @@
         <v>90</v>
       </c>
       <c r="B138" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C138" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
@@ -69572,117 +69596,117 @@
         <v>94</v>
       </c>
       <c r="B139" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C139" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>559</v>
+      <c r="A140">
+        <v>98</v>
       </c>
       <c r="B140" t="s">
-        <v>359</v>
-      </c>
-      <c r="C140">
-        <v>0</v>
+        <v>630</v>
+      </c>
+      <c r="C140" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B141" t="s">
-        <v>532</v>
+        <v>631</v>
       </c>
       <c r="C141" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B142" t="s">
-        <v>533</v>
+        <v>632</v>
       </c>
       <c r="C142" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>560</v>
+      <c r="A143">
+        <v>110</v>
       </c>
       <c r="B143" t="s">
-        <v>359</v>
-      </c>
-      <c r="C143">
-        <v>0</v>
+        <v>633</v>
+      </c>
+      <c r="C143" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B144" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C144" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="B145" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="C145" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
-        <v>561</v>
+      <c r="A146">
+        <v>122</v>
       </c>
       <c r="B146" t="s">
-        <v>354</v>
-      </c>
-      <c r="C146">
-        <v>0</v>
+        <v>634</v>
+      </c>
+      <c r="C146" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="B147" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C147" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="B148" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="C148" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>562</v>
+        <v>625</v>
       </c>
       <c r="B149" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="C149">
         <v>0</v>
@@ -69690,497 +69714,574 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="B150" t="s">
-        <v>538</v>
+        <v>626</v>
       </c>
       <c r="C150" t="s">
-        <v>553</v>
+        <v>635</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151">
-        <v>170</v>
+      <c r="A151" t="s">
+        <v>637</v>
       </c>
       <c r="B151" t="s">
-        <v>539</v>
-      </c>
-      <c r="C151" t="s">
-        <v>547</v>
+        <v>359</v>
+      </c>
+      <c r="C151">
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="B152" t="s">
-        <v>540</v>
+        <v>636</v>
       </c>
       <c r="C152" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="B153" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="C153" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="B154" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="C154" t="s">
-        <v>631</v>
+        <v>545</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B155" t="s">
-        <v>543</v>
+        <v>638</v>
       </c>
       <c r="C155" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A156">
-        <v>190</v>
+      <c r="A156" t="s">
+        <v>639</v>
       </c>
       <c r="B156" t="s">
-        <v>544</v>
-      </c>
-      <c r="C156" t="s">
-        <v>556</v>
+        <v>354</v>
+      </c>
+      <c r="C156">
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B157" t="s">
-        <v>545</v>
+        <v>536</v>
       </c>
       <c r="C157" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="B158" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
       <c r="C158" t="s">
-        <v>563</v>
+        <v>545</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159">
-        <v>202</v>
+        <v>174</v>
       </c>
       <c r="B159" t="s">
-        <v>354</v>
-      </c>
-      <c r="C159">
-        <v>0</v>
+        <v>538</v>
+      </c>
+      <c r="C159" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160">
+        <v>178</v>
+      </c>
+      <c r="B160" t="s">
+        <v>539</v>
+      </c>
+      <c r="C160" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>182</v>
+      </c>
+      <c r="B161" t="s">
+        <v>540</v>
+      </c>
+      <c r="C161" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>186</v>
+      </c>
+      <c r="B162" t="s">
+        <v>541</v>
+      </c>
+      <c r="C162" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>190</v>
+      </c>
+      <c r="B163" t="s">
+        <v>542</v>
+      </c>
+      <c r="C163" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>194</v>
+      </c>
+      <c r="B164" t="s">
+        <v>543</v>
+      </c>
+      <c r="C164" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>198</v>
+      </c>
+      <c r="B165" t="s">
+        <v>544</v>
+      </c>
+      <c r="C165" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>202</v>
+      </c>
+      <c r="B166" t="s">
+        <v>354</v>
+      </c>
+      <c r="C166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167">
         <v>203</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B167" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A161">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168">
         <v>204</v>
-      </c>
-      <c r="B161" t="s">
-        <v>354</v>
-      </c>
-      <c r="C161">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" ht="21" x14ac:dyDescent="0.4">
-      <c r="A164" s="7" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A166" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A167">
-        <v>0</v>
-      </c>
-      <c r="B167" t="s">
-        <v>354</v>
-      </c>
-      <c r="C167">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A168">
-        <v>1</v>
       </c>
       <c r="B168" t="s">
         <v>354</v>
       </c>
       <c r="C168">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A169">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="A171" s="7" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>0</v>
+      </c>
+      <c r="B174" t="s">
+        <v>354</v>
+      </c>
+      <c r="C174">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>1</v>
+      </c>
+      <c r="B175" t="s">
+        <v>354</v>
+      </c>
+      <c r="C175">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176">
         <v>2</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B176" t="s">
         <v>354</v>
       </c>
-      <c r="C169">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A170">
-        <v>3</v>
-      </c>
-      <c r="B170" t="s">
-        <v>354</v>
-      </c>
-      <c r="C170">
-        <v>1</v>
-      </c>
-      <c r="D170" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A171">
-        <v>4</v>
-      </c>
-      <c r="B171" t="s">
-        <v>354</v>
-      </c>
-      <c r="C171">
-        <v>39</v>
-      </c>
-      <c r="D171" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A172">
-        <v>5</v>
-      </c>
-      <c r="B172" t="s">
-        <v>354</v>
-      </c>
-      <c r="C172">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A173">
-        <v>6</v>
-      </c>
-      <c r="B173" t="s">
-        <v>493</v>
-      </c>
-      <c r="C173" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A174">
-        <v>10</v>
-      </c>
-      <c r="B174" t="s">
-        <v>494</v>
-      </c>
-      <c r="C174" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A175">
-        <v>14</v>
-      </c>
-      <c r="B175" t="s">
-        <v>495</v>
-      </c>
-      <c r="C175" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A176">
-        <v>18</v>
-      </c>
-      <c r="B176" t="s">
-        <v>496</v>
-      </c>
-      <c r="C176" t="s">
-        <v>583</v>
+      <c r="C176">
+        <v>22</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B177" t="s">
-        <v>497</v>
-      </c>
-      <c r="C177" t="s">
-        <v>584</v>
+        <v>354</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
+      <c r="D177" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B178" t="s">
-        <v>498</v>
-      </c>
-      <c r="C178" t="s">
-        <v>585</v>
+        <v>354</v>
+      </c>
+      <c r="C178">
+        <v>39</v>
+      </c>
+      <c r="D178" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B179" t="s">
-        <v>499</v>
-      </c>
-      <c r="C179" t="s">
-        <v>586</v>
+        <v>354</v>
+      </c>
+      <c r="C179">
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="B180" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="C180" t="s">
-        <v>587</v>
+        <v>573</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B181" t="s">
-        <v>588</v>
+        <v>492</v>
       </c>
       <c r="C181" t="s">
-        <v>547</v>
+        <v>574</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B182" t="s">
-        <v>360</v>
+        <v>493</v>
+      </c>
+      <c r="C182" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B183" t="s">
-        <v>354</v>
-      </c>
-      <c r="C183">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" ht="21" x14ac:dyDescent="0.4">
-      <c r="A186" s="7" t="s">
-        <v>409</v>
+        <v>494</v>
+      </c>
+      <c r="C183" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A184">
+        <v>22</v>
+      </c>
+      <c r="B184" t="s">
+        <v>495</v>
+      </c>
+      <c r="C184" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A185">
+        <v>26</v>
+      </c>
+      <c r="B185" t="s">
+        <v>496</v>
+      </c>
+      <c r="C185" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <v>30</v>
+      </c>
+      <c r="B186" t="s">
+        <v>497</v>
+      </c>
+      <c r="C186" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <v>34</v>
+      </c>
+      <c r="B187" t="s">
+        <v>498</v>
+      </c>
+      <c r="C187" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A188" t="s">
-        <v>353</v>
+      <c r="A188">
+        <v>38</v>
+      </c>
+      <c r="B188" t="s">
+        <v>581</v>
+      </c>
+      <c r="C188" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B189" t="s">
-        <v>354</v>
-      </c>
-      <c r="C189">
-        <v>22</v>
+        <v>360</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="B190" t="s">
         <v>354</v>
       </c>
       <c r="C190">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A191">
-        <v>2</v>
-      </c>
-      <c r="B191" t="s">
-        <v>354</v>
-      </c>
-      <c r="C191">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A192">
-        <v>3</v>
-      </c>
-      <c r="B192" t="s">
-        <v>354</v>
-      </c>
-      <c r="C192">
-        <v>2</v>
-      </c>
-      <c r="D192" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A193">
-        <v>4</v>
-      </c>
-      <c r="B193" t="s">
-        <v>354</v>
-      </c>
-      <c r="C193">
-        <v>29</v>
-      </c>
-      <c r="D193" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A194">
-        <v>5</v>
-      </c>
-      <c r="B194" t="s">
-        <v>354</v>
-      </c>
-      <c r="C194">
-        <v>1</v>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="21" x14ac:dyDescent="0.4">
+      <c r="A193" s="7" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A195">
-        <v>6</v>
-      </c>
-      <c r="B195" t="s">
-        <v>493</v>
-      </c>
-      <c r="C195" t="s">
-        <v>589</v>
+      <c r="A195" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B196" t="s">
-        <v>494</v>
-      </c>
-      <c r="C196" t="s">
-        <v>590</v>
+        <v>354</v>
+      </c>
+      <c r="C196">
+        <v>22</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B197" t="s">
-        <v>495</v>
-      </c>
-      <c r="C197" t="s">
-        <v>591</v>
+        <v>354</v>
+      </c>
+      <c r="C197">
+        <v>22</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B198" t="s">
-        <v>496</v>
-      </c>
-      <c r="C198" t="s">
-        <v>592</v>
+        <v>354</v>
+      </c>
+      <c r="C198">
+        <v>22</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B199" t="s">
-        <v>497</v>
-      </c>
-      <c r="C199" t="s">
-        <v>593</v>
+        <v>354</v>
+      </c>
+      <c r="C199">
+        <v>2</v>
+      </c>
+      <c r="D199" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A200" t="s">
-        <v>594</v>
+      <c r="A200">
+        <v>4</v>
       </c>
       <c r="B200" t="s">
-        <v>359</v>
-      </c>
-      <c r="C200" t="s">
-        <v>595</v>
+        <v>354</v>
+      </c>
+      <c r="C200">
+        <v>29</v>
+      </c>
+      <c r="D200" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B201" t="s">
-        <v>360</v>
+        <v>354</v>
+      </c>
+      <c r="C201">
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202">
+        <v>6</v>
+      </c>
+      <c r="B202" t="s">
+        <v>491</v>
+      </c>
+      <c r="C202" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A203">
+        <v>10</v>
+      </c>
+      <c r="B203" t="s">
+        <v>492</v>
+      </c>
+      <c r="C203" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A204">
+        <v>14</v>
+      </c>
+      <c r="B204" t="s">
+        <v>493</v>
+      </c>
+      <c r="C204" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A205">
+        <v>18</v>
+      </c>
+      <c r="B205" t="s">
+        <v>494</v>
+      </c>
+      <c r="C205" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A206">
+        <v>22</v>
+      </c>
+      <c r="B206" t="s">
+        <v>495</v>
+      </c>
+      <c r="C206" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>587</v>
+      </c>
+      <c r="B207" t="s">
+        <v>359</v>
+      </c>
+      <c r="C207" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A208">
+        <v>32</v>
+      </c>
+      <c r="B208" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A209">
         <v>33</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B209" t="s">
         <v>354</v>
       </c>
-      <c r="C202">
+      <c r="C209">
         <v>255</v>
       </c>
     </row>
@@ -70205,7 +70306,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -70215,7 +70316,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -70225,100 +70326,100 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B9" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C9" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B10" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C10" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B11" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C11" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C12" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B13" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C13" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B14" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C14" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B15" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C15" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B16" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C16" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -70329,7 +70430,7 @@
         <v>340</v>
       </c>
       <c r="C17" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -70340,418 +70441,418 @@
         <v>340</v>
       </c>
       <c r="C18" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B19" t="s">
         <v>357</v>
       </c>
       <c r="C19" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B20" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="C20" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B21" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
       <c r="C21" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B22" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
       <c r="C22" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B23" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="C23" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B24" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="C24" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B25" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C25" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B26" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C26" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B27" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C27" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B28" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C28" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B29" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C29" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B30" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C30" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B31" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C31" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B32" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C32" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B33" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C33" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B34" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C34" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B35" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C35" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B36" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C36" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B37" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C37" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B38" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C38" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B39" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C39" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B40" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C40" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B41" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C41" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B42" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C42" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B43" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C43" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B44" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C44" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B45" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C45" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B46" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C46" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B47" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C47" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B48" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C48" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B49" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C49" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B50" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C50" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B51" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C51" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B52" t="s">
+        <v>599</v>
+      </c>
+      <c r="C52" t="s">
         <v>606</v>
-      </c>
-      <c r="C52" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B53" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C53" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B54" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C54" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>